<commit_message>
Finalização da base de dados
</commit_message>
<xml_diff>
--- a/Coleta/base.xlsx
+++ b/Coleta/base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alinsperedu-my.sharepoint.com/personal/jonasbp_al_insper_edu_br/Documents/2021.2/Ciência dos Dados/P1/Backup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="555" documentId="11_4A969315AC439293EE75102ED759FC45E12C451E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A26DC59E-4ED4-684A-8306-150097FFF929}"/>
+  <xr:revisionPtr revIDLastSave="565" documentId="11_4A969315AC439293EE75102ED759FC45E12C451E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9344FBD-21EF-0045-98AD-101BFFF765DA}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="32000" windowHeight="15780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="418">
   <si>
     <t>Treinamento</t>
   </si>
@@ -766,144 +766,27 @@
     <t>alexa play digital dash</t>
   </si>
   <si>
-    <t>tenha calma com a alexa vitu! https://t.co/9ryct9qpv6 via @youtube</t>
-  </si>
-  <si>
-    <t>@lovsesteves @favsztar @tarxio eu nessa sala gritaria: alexa toca lady gaga</t>
-  </si>
-  <si>
-    <t>#aprizionradio aqui tem #rock #anos80 #anos90 de ultraje a rigor, ultraje a rigor e barão vermelho. na alexa ou google nest, diga: "ouvir rock verde amarelo no tunein" ou clique direto para ouvir! https://t.co/qqymwnwm6j</t>
-  </si>
-  <si>
-    <t>@alexa_sasmaz_ eu fui correndo no youtube ver, quando vi que não tinha outro fiquei triste. enfim, a inocente kkkkkkkkkkkkkkkk</t>
-  </si>
-  <si>
-    <t>@_gabomontalvo alexa😎</t>
-  </si>
-  <si>
-    <t>@alexa_rojas04 chula🥰</t>
-  </si>
-  <si>
-    <t>perdi a hora das crianças irem pra escola hoje...
-8h35 - malu correndo atrás do caio chamando ele de fdp
-8h50 - caio tacando a cozinha de brinquedo da malu nas costas dela
-9h09 - malu tacando vitamina na alexa e levando pro banheiro pra lavar
-sextou....</t>
-  </si>
-  <si>
-    <t>“a evolução dos smartspeakers passará por três fases: nascimento (alexa surgiu em 2014), maturação e socialização (extensão do uso). [...] estamos na transição do mobile first para o voice first.” - andoni orrantia</t>
-  </si>
-  <si>
-    <t>humm alexa com r$ 100 de desconto 
-https://t.co/qoxhmqlocs https://t.co/uj3tvh9mdw</t>
-  </si>
-  <si>
-    <t>@iamcindyr__ alexa: 😆 https://t.co/azup6hwjs4</t>
-  </si>
-  <si>
-    <t>eu vi o meu pai não faz nem 5 horas atrás e já to chorando de sdd          alexa play mommy* issues</t>
-  </si>
-  <si>
-    <t>alexa show me a kapenta @tanaka_power_  🤣🤣🤣🤣🤣 https://t.co/1wvdcffjmm</t>
-  </si>
-  <si>
-    <t>+1 dia de estágio 🥲</t>
-  </si>
-  <si>
     <t>é mt engraçado ouvir os vizinhos falando c a alexa me sinto em black mirror seila</t>
   </si>
   <si>
-    <t>o boletim de notícias da dw é disponibilizado de segunda a sexta-feira, em duas edições diárias, de manhã e à tarde, pelo spotify (https://t.co/97dlgjw1ry), deezer, youtube, apple podcasts, google podcasts, alexa, google assistente e google home: https://t.co/xvftgjavcl</t>
-  </si>
-  <si>
     <t>muito bom conversar com a alexa</t>
   </si>
   <si>
-    <t>é pedi demais ter esses dois como meus motoristas?? https://t.co/iy69bewguw</t>
-  </si>
-  <si>
-    <t>preciso de alguém pra conversar sobre alexa e kaite urgente</t>
-  </si>
-  <si>
-    <t>@yujinkoomios alexa</t>
-  </si>
-  <si>
-    <t>@alexa_bispo delicia de bombom</t>
-  </si>
-  <si>
-    <t>@alnapox alexa</t>
-  </si>
-  <si>
-    <t>@alexa_fcp oi! tudo bem? :) 
-sempre que quiser, o código de consultora "lari" dá 10% de desconto no site e app da c&amp;amp;a 🤩
-não é cumulativo com cupom, mas me ajuda muuuuito se usar 💛
-*produtos vendidos e entregues pela c&amp;amp;a, menos eletrônicos</t>
-  </si>
-  <si>
     <t>perguntei pra alexa se podia chamar ela de jarvis e ela disse não to triste</t>
   </si>
   <si>
-    <t>#aprizionradio aqui tem #rock #anos80 #anos90 de gang 90 &amp;amp; absurdetes, titãs e violator. na alexa ou google nest, diga: "ouvir rock verde amarelo no tunein" ou clique direto para ouvir! https://t.co/qqymwnwm6j</t>
-  </si>
-  <si>
     <t>minha vizinho 8 da manhã com sertanejo (eu odeio), da cama só falei “alexa pet shop boys”</t>
   </si>
   <si>
-    <t>@pandadelamaldad panda representa al fandom 🤭🤭</t>
-  </si>
-  <si>
-    <t>@luansantosti @vquaiato py é uma delicinha.
-tô batendo cabeça tentando desenvolver uma skill da alexa.
-mudar o canal do iptv pela alexa vai ficar muito iron man kkk</t>
-  </si>
-  <si>
     <t>e a alexa que tá fazendo elogios antes de dar boa noite agora? seria esse o #setembroamarelo da @amazonbr ? achei inesperadamente fofo 🥰</t>
   </si>
   <si>
-    <t>alexa, o novo pesadelo da @hey_mika https://t.co/1whfm1g7ff</t>
-  </si>
-  <si>
-    <t>agora ir pra onde?? bursa mesmo ? e as tias chatas? https://t.co/bs6vt8bodx</t>
-  </si>
-  <si>
-    <t>@alexacord_ @wallywest1987 @_vinnygomes12 @1fernandoreal @g1 alexa, qual a altura do monte everest?</t>
-  </si>
-  <si>
-    <t>@vitucs pensa pelo lado bom agora vc vai ter uma alexa pra conversar hahahahaha!</t>
-  </si>
-  <si>
-    <t>comecar a comprar roupa 💆🏻‍♀️ quero msm conseguir mudar o meu estilo</t>
-  </si>
-  <si>
-    <t>@sorn_wcast -alexa</t>
-  </si>
-  <si>
-    <t>caralho, alguém falou alexa na tv e a minha respondeu altão do meu lado eu tomei um susto</t>
-  </si>
-  <si>
-    <t>@alexa_sasmaz_ só os şaşman pra me fazer ver dizi em andamento, que carai de homem bonito</t>
-  </si>
-  <si>
-    <t>@othiagonobre @belafeitosaa para gente! não gosto de casal….. 
-alexa play good 4 you by olivia rodrigo minute 0:39</t>
-  </si>
-  <si>
-    <t>pelo menos comprei uns botins finalmente</t>
-  </si>
-  <si>
     <t>alexa toca nobody em loop por 48 horas seguidas</t>
   </si>
   <si>
     <t>a alexa dizendo pra eu tomar meu floral e eu ouvindo enquanto como uma torta holandesa de café da manhã https://t.co/ryawaayscm</t>
   </si>
   <si>
-    <t>@nourdalgos modern family é minha fav da vida!!! alexa &amp;amp; katie mt boa tb nunca vi ninguem q era fa por aquii</t>
-  </si>
-  <si>
-    <t>@gillespieness @dearcharlison sim!!!
-ps: adorei o vídeo 💜</t>
-  </si>
-  <si>
     <t>cheguei na minha avó e ela torando essa na alexa enquanto acende um cigarro  https://t.co/lrbgggcblw</t>
   </si>
   <si>
@@ -913,64 +796,16 @@
     <t>alexa, faz um cafuné</t>
   </si>
   <si>
-    <t>@noshyoon1 @ocleitonsilva3 @heavmetalover @tempestvic @vinilag @viniciuszeira @bchartsnet é da rádio moldou uma geração indie</t>
-  </si>
-  <si>
-    <t>tô apaixonada nesse edit com os outros personagens do aytaç e da cemre como casais ❤️🥺 vontade de guarda em um potinho🥺 espero que não flope https://t.co/y3a0rzgtnh</t>
-  </si>
-  <si>
-    <t>@alexa_petit_ sofrer sozinha é muito difícil 😔</t>
-  </si>
-  <si>
-    <t>• day seven🦋
-• momento inspirador🦋
-o momento inspirador para mim, foi em wake up. a julie conseguiu encarar o medo, conseguiu cantar depois de tanto tempo. ela finalmente deu uma chance para ela mesma. como ela fala na música, ela usou a dor dela, porque faz parte dela.🦋 https://t.co/tmz8cwqz6n</t>
-  </si>
-  <si>
-    <t>@mookheewin pois é se ela for continua em i̇stambul que seja com a selin</t>
-  </si>
-  <si>
     <t>alexa acordou bem hoje 🥰🥰🥰🥰 https://t.co/60855zxdu2</t>
   </si>
   <si>
-    <t>@alexa_sasmaz_ o emre é de qual dizi?</t>
-  </si>
-  <si>
-    <t>echo dot 3ª geração smart speaker com alexa - amazon
-por r$ 229,90!
-✨ link: https://t.co/dojjuh93rf https://t.co/csnt9ztw9x</t>
-  </si>
-  <si>
-    <t>#aprizionradio aqui tem #rock #anos80 #anos90 de biquini cavadão, leoni e ratos de porão. na alexa ou google nest, diga: "ouvir rock verde amarelo no tunein" ou clique direto para ouvir! https://t.co/qqymwnwm6j</t>
-  </si>
-  <si>
     <t>minha alexa me sacaneou, acendeu a luz na minha cara de madrugada</t>
   </si>
   <si>
-    <t>@kpophappenings_ alexa? :))
-https://t.co/1qof50v0rq</t>
-  </si>
-  <si>
-    <t>@flavisonlima kkkkk fiquei c ódio de mim, que só entendi o real motivo da alexa existir, a pouco tempo.</t>
-  </si>
-  <si>
-    <t>@alexa_sasmaz_ alexa tenha piedade se faz favor amiga
-isso não se faz</t>
-  </si>
-  <si>
-    <t>alexa vai apresentar o bbb em inovadora parceria da globo com a amazon.</t>
-  </si>
-  <si>
     <t>próxima vez que eu pedir música pra alexa tocar e ela vier com giulia be eu jogo fora</t>
   </si>
   <si>
-    <t>eu nao tenho alexa</t>
-  </si>
-  <si>
     <t>eu amo o conhecimento inútil que aprendo com a alexa</t>
-  </si>
-  <si>
-    <t>@jatpbr @shinesjuke1 feliz um ano portal!!!💜👻🦋🎸</t>
   </si>
   <si>
     <t>meu pai comprou uma alexa, agora o resto vcs já imaginam😂😂😂</t>
@@ -1532,6 +1367,41 @@
   </si>
   <si>
     <t>alexa, da mis clases híbridas.</t>
+  </si>
+  <si>
+    <t>eu vou ser mt nerdola se eu fazer rotinas na minha alexa com tema de star trek???????</t>
+  </si>
+  <si>
+    <t>alexa me recomendou a playlist rock party e eu tinha me esquecido de como é bom ouvir rock</t>
+  </si>
+  <si>
+    <t>hoje a alexa me acordou com wow do loona gente eu quase pulei da cama o susto que eu levei foi bem no refrão https://t.co/w4csmpvtde</t>
+  </si>
+  <si>
+    <t>alexa, toque as mais tristes do frank ocean</t>
+  </si>
+  <si>
+    <t>alexa play paranoia by jay b</t>
+  </si>
+  <si>
+    <t>xinguei tanto minha alexa que ela parou de me responder tadinha</t>
+  </si>
+  <si>
+    <t>eu: alexa, toca gungor 
+alexa: tocando as músicas de gugu no spotify</t>
+  </si>
+  <si>
+    <t>alexa, dá essa aula pra mim faz favor</t>
+  </si>
+  <si>
+    <t>gente acabei de descobrir que se tu pedir da alexa pra rezar o terço contigo ela reza
+vou comprar uma alexa agora</t>
+  </si>
+  <si>
+    <t>toda vez que eu peço pra alexa colocar na lista de compras molho shoyu e ela responde "adicionei molho shoyu" eu fico pensando na passivo-agressividade dela em me responder com a pronúncia correta em japonês</t>
+  </si>
+  <si>
+    <t>“alexa toque uma playlist de shrek” advinha que disse isso 😂😂</t>
   </si>
 </sst>
 </file>
@@ -1555,7 +1425,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1571,6 +1441,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1602,7 +1478,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1615,6 +1491,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2707,7 +2584,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
-        <v>412</v>
+        <v>363</v>
       </c>
       <c r="B94" s="3">
         <v>1</v>
@@ -2731,7 +2608,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
-        <v>413</v>
+        <v>364</v>
       </c>
       <c r="B97" s="3">
         <v>1</v>
@@ -2739,7 +2616,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="B98" s="3">
         <v>1</v>
@@ -2747,7 +2624,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
-        <v>250</v>
+        <v>230</v>
       </c>
       <c r="B99" s="3">
         <v>1</v>
@@ -2755,7 +2632,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
-        <v>252</v>
+        <v>231</v>
       </c>
       <c r="B100" s="3">
         <v>1</v>
@@ -2763,7 +2640,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
-        <v>414</v>
+        <v>365</v>
       </c>
       <c r="B101" s="3">
         <v>1</v>
@@ -2771,7 +2648,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
-        <v>266</v>
+        <v>233</v>
       </c>
       <c r="B102" s="3">
         <v>1</v>
@@ -2779,7 +2656,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
-        <v>267</v>
+        <v>234</v>
       </c>
       <c r="B103" s="3">
         <v>1</v>
@@ -2787,7 +2664,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
-        <v>415</v>
+        <v>366</v>
       </c>
       <c r="B104" s="3">
         <v>1</v>
@@ -2795,7 +2672,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
-        <v>271</v>
+        <v>236</v>
       </c>
       <c r="B105" s="3">
         <v>1</v>
@@ -2803,7 +2680,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
-        <v>272</v>
+        <v>237</v>
       </c>
       <c r="B106" s="3">
         <v>1</v>
@@ -2811,7 +2688,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
-        <v>416</v>
+        <v>367</v>
       </c>
       <c r="B107" s="3">
         <v>1</v>
@@ -2819,7 +2696,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
-        <v>278</v>
+        <v>238</v>
       </c>
       <c r="B108" s="3">
         <v>1</v>
@@ -2827,7 +2704,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
-        <v>417</v>
+        <v>368</v>
       </c>
       <c r="B109" s="3">
         <v>1</v>
@@ -2835,7 +2712,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
-        <v>282</v>
+        <v>239</v>
       </c>
       <c r="B110" s="3">
         <v>1</v>
@@ -2843,7 +2720,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
-        <v>287</v>
+        <v>240</v>
       </c>
       <c r="B111" s="3">
         <v>1</v>
@@ -2851,7 +2728,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
-        <v>289</v>
+        <v>241</v>
       </c>
       <c r="B112" s="3">
         <v>1</v>
@@ -2859,7 +2736,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
-        <v>291</v>
+        <v>242</v>
       </c>
       <c r="B113" s="3">
         <v>1</v>
@@ -2867,7 +2744,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
-        <v>418</v>
+        <v>369</v>
       </c>
       <c r="B114" s="3">
         <v>1</v>
@@ -2875,7 +2752,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
-        <v>419</v>
+        <v>370</v>
       </c>
       <c r="B115" s="3">
         <v>1</v>
@@ -2883,7 +2760,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
-        <v>420</v>
+        <v>371</v>
       </c>
       <c r="B116" s="3">
         <v>1</v>
@@ -2891,7 +2768,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
-        <v>293</v>
+        <v>244</v>
       </c>
       <c r="B117" s="3">
         <v>1</v>
@@ -2899,7 +2776,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
-        <v>421</v>
+        <v>372</v>
       </c>
       <c r="B118" s="3">
         <v>1</v>
@@ -2907,7 +2784,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
-        <v>297</v>
+        <v>248</v>
       </c>
       <c r="B119" s="3">
         <v>1</v>
@@ -2915,7 +2792,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
-        <v>301</v>
+        <v>252</v>
       </c>
       <c r="B120" s="3">
         <v>1</v>
@@ -2923,7 +2800,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
-        <v>422</v>
+        <v>373</v>
       </c>
       <c r="B121" s="3">
         <v>1</v>
@@ -2931,7 +2808,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
-        <v>423</v>
+        <v>374</v>
       </c>
       <c r="B122" s="3">
         <v>1</v>
@@ -2939,7 +2816,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
-        <v>317</v>
+        <v>268</v>
       </c>
       <c r="B123" s="3">
         <v>1</v>
@@ -2947,7 +2824,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
-        <v>323</v>
+        <v>274</v>
       </c>
       <c r="B124" s="3">
         <v>1</v>
@@ -2955,7 +2832,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
-        <v>322</v>
+        <v>273</v>
       </c>
       <c r="B125" s="3">
         <v>1</v>
@@ -2963,7 +2840,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
-        <v>326</v>
+        <v>277</v>
       </c>
       <c r="B126" s="3">
         <v>1</v>
@@ -2971,7 +2848,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
-        <v>329</v>
+        <v>280</v>
       </c>
       <c r="B127" s="3">
         <v>1</v>
@@ -2979,7 +2856,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
-        <v>328</v>
+        <v>279</v>
       </c>
       <c r="B128" s="3">
         <v>1</v>
@@ -2987,7 +2864,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="s">
-        <v>424</v>
+        <v>375</v>
       </c>
       <c r="B129" s="3">
         <v>1</v>
@@ -2995,7 +2872,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
-        <v>425</v>
+        <v>376</v>
       </c>
       <c r="B130" s="3">
         <v>1</v>
@@ -3003,7 +2880,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
-        <v>330</v>
+        <v>281</v>
       </c>
       <c r="B131" s="3">
         <v>1</v>
@@ -3011,7 +2888,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
-        <v>426</v>
+        <v>377</v>
       </c>
       <c r="B132" s="3">
         <v>1</v>
@@ -3019,7 +2896,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
-        <v>335</v>
+        <v>286</v>
       </c>
       <c r="B133" s="3">
         <v>1</v>
@@ -3027,7 +2904,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
-        <v>336</v>
+        <v>287</v>
       </c>
       <c r="B134" s="3">
         <v>1</v>
@@ -3035,7 +2912,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
-        <v>427</v>
+        <v>378</v>
       </c>
       <c r="B135" s="3">
         <v>1</v>
@@ -3043,7 +2920,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" s="3" t="s">
-        <v>428</v>
+        <v>379</v>
       </c>
       <c r="B136" s="3">
         <v>1</v>
@@ -3051,7 +2928,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" s="3" t="s">
-        <v>345</v>
+        <v>296</v>
       </c>
       <c r="B137" s="3">
         <v>1</v>
@@ -3059,7 +2936,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" s="3" t="s">
-        <v>429</v>
+        <v>380</v>
       </c>
       <c r="B138" s="3">
         <v>1</v>
@@ -3067,7 +2944,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" s="3" t="s">
-        <v>363</v>
+        <v>314</v>
       </c>
       <c r="B139" s="3">
         <v>1</v>
@@ -3075,7 +2952,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" s="3" t="s">
-        <v>365</v>
+        <v>316</v>
       </c>
       <c r="B140" s="3">
         <v>1</v>
@@ -3083,7 +2960,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" s="3" t="s">
-        <v>367</v>
+        <v>318</v>
       </c>
       <c r="B141" s="3">
         <v>1</v>
@@ -3091,7 +2968,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" s="3" t="s">
-        <v>374</v>
+        <v>325</v>
       </c>
       <c r="B142" s="3">
         <v>1</v>
@@ -3099,7 +2976,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" s="3" t="s">
-        <v>430</v>
+        <v>381</v>
       </c>
       <c r="B143" s="3">
         <v>1</v>
@@ -3107,7 +2984,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" s="3" t="s">
-        <v>431</v>
+        <v>382</v>
       </c>
       <c r="B144" s="3">
         <v>1</v>
@@ -3115,7 +2992,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" s="3" t="s">
-        <v>432</v>
+        <v>383</v>
       </c>
       <c r="B145" s="3">
         <v>1</v>
@@ -3123,7 +3000,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" s="3" t="s">
-        <v>433</v>
+        <v>384</v>
       </c>
       <c r="B146" s="3">
         <v>1</v>
@@ -3131,7 +3008,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" s="3" t="s">
-        <v>434</v>
+        <v>385</v>
       </c>
       <c r="B147" s="3">
         <v>1</v>
@@ -3139,7 +3016,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" s="3" t="s">
-        <v>384</v>
+        <v>335</v>
       </c>
       <c r="B148" s="3">
         <v>1</v>
@@ -3147,7 +3024,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" s="3" t="s">
-        <v>435</v>
+        <v>386</v>
       </c>
       <c r="B149" s="3">
         <v>1</v>
@@ -3155,7 +3032,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" s="3" t="s">
-        <v>436</v>
+        <v>387</v>
       </c>
       <c r="B150" s="3">
         <v>1</v>
@@ -3163,7 +3040,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" s="3" t="s">
-        <v>437</v>
+        <v>388</v>
       </c>
       <c r="B151" s="3">
         <v>1</v>
@@ -4235,7 +4112,7 @@
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A285" s="4" t="s">
-        <v>446</v>
+        <v>397</v>
       </c>
       <c r="B285" s="5">
         <v>0</v>
@@ -4243,7 +4120,7 @@
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A286" s="4" t="s">
-        <v>447</v>
+        <v>398</v>
       </c>
       <c r="B286" s="5">
         <v>0</v>
@@ -4251,7 +4128,7 @@
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A287" s="4" t="s">
-        <v>448</v>
+        <v>399</v>
       </c>
       <c r="B287" s="5">
         <v>0</v>
@@ -4259,7 +4136,7 @@
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A288" s="4" t="s">
-        <v>449</v>
+        <v>400</v>
       </c>
       <c r="B288" s="5">
         <v>0</v>
@@ -4283,7 +4160,7 @@
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A291" s="4" t="s">
-        <v>450</v>
+        <v>401</v>
       </c>
       <c r="B291" s="5">
         <v>0</v>
@@ -4307,7 +4184,7 @@
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A294" s="4" t="s">
-        <v>451</v>
+        <v>402</v>
       </c>
       <c r="B294" s="5">
         <v>0</v>
@@ -4323,7 +4200,7 @@
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A296" s="4" t="s">
-        <v>452</v>
+        <v>403</v>
       </c>
       <c r="B296" s="5">
         <v>0</v>
@@ -4339,7 +4216,7 @@
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A298" s="4" t="s">
-        <v>453</v>
+        <v>404</v>
       </c>
       <c r="B298" s="5">
         <v>0</v>
@@ -4347,7 +4224,7 @@
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A299" s="4" t="s">
-        <v>454</v>
+        <v>405</v>
       </c>
       <c r="B299" s="5">
         <v>0</v>
@@ -4363,7 +4240,7 @@
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A301" s="4" t="s">
-        <v>455</v>
+        <v>406</v>
       </c>
       <c r="B301" s="5">
         <v>0</v>
@@ -4399,8 +4276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4431,7 +4308,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
@@ -4439,7 +4316,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>250</v>
+        <v>230</v>
       </c>
       <c r="B5" s="3">
         <v>1</v>
@@ -4447,7 +4324,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>255</v>
+        <v>232</v>
       </c>
       <c r="B6" s="3">
         <v>1</v>
@@ -4455,7 +4332,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>266</v>
+        <v>233</v>
       </c>
       <c r="B7" s="3">
         <v>1</v>
@@ -4463,7 +4340,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>267</v>
+        <v>234</v>
       </c>
       <c r="B8" s="3">
         <v>1</v>
@@ -4471,7 +4348,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>270</v>
+        <v>235</v>
       </c>
       <c r="B9" s="3">
         <v>1</v>
@@ -4479,7 +4356,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>271</v>
+        <v>236</v>
       </c>
       <c r="B10" s="3">
         <v>1</v>
@@ -4487,7 +4364,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>272</v>
+        <v>237</v>
       </c>
       <c r="B11" s="3">
         <v>1</v>
@@ -4495,7 +4372,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>282</v>
+        <v>239</v>
       </c>
       <c r="B12" s="3">
         <v>1</v>
@@ -4503,7 +4380,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>287</v>
+        <v>240</v>
       </c>
       <c r="B13" s="3">
         <v>1</v>
@@ -4511,7 +4388,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>289</v>
+        <v>241</v>
       </c>
       <c r="B14" s="3">
         <v>1</v>
@@ -4519,7 +4396,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>291</v>
+        <v>242</v>
       </c>
       <c r="B15" s="3">
         <v>1</v>
@@ -4527,7 +4404,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>293</v>
+        <v>244</v>
       </c>
       <c r="B16" s="3">
         <v>1</v>
@@ -4535,7 +4412,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>297</v>
+        <v>248</v>
       </c>
       <c r="B17" s="3">
         <v>1</v>
@@ -4543,7 +4420,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>301</v>
+        <v>252</v>
       </c>
       <c r="B18" s="3">
         <v>1</v>
@@ -4551,7 +4428,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>322</v>
+        <v>273</v>
       </c>
       <c r="B19" s="3">
         <v>1</v>
@@ -4559,7 +4436,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>326</v>
+        <v>277</v>
       </c>
       <c r="B20" s="3">
         <v>1</v>
@@ -4567,7 +4444,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>329</v>
+        <v>280</v>
       </c>
       <c r="B21" s="3">
         <v>1</v>
@@ -4575,7 +4452,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>336</v>
+        <v>287</v>
       </c>
       <c r="B22" s="3">
         <v>1</v>
@@ -4583,7 +4460,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>337</v>
+        <v>288</v>
       </c>
       <c r="B23" s="3">
         <v>1</v>
@@ -4591,7 +4468,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>345</v>
+        <v>296</v>
       </c>
       <c r="B24" s="3">
         <v>1</v>
@@ -4599,7 +4476,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>349</v>
+        <v>300</v>
       </c>
       <c r="B25" s="3">
         <v>1</v>
@@ -4607,7 +4484,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>367</v>
+        <v>318</v>
       </c>
       <c r="B26" s="3">
         <v>1</v>
@@ -4615,7 +4492,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>374</v>
+        <v>325</v>
       </c>
       <c r="B27" s="3">
         <v>1</v>
@@ -4623,7 +4500,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>387</v>
+        <v>338</v>
       </c>
       <c r="B28" s="3">
         <v>1</v>
@@ -4631,7 +4508,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>406</v>
+        <v>357</v>
       </c>
       <c r="B29" s="3">
         <v>1</v>
@@ -4639,7 +4516,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>411</v>
+        <v>362</v>
       </c>
       <c r="B30" s="3">
         <v>1</v>
@@ -4647,7 +4524,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>387</v>
+        <v>338</v>
       </c>
       <c r="B31" s="3">
         <v>1</v>
@@ -4655,7 +4532,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>438</v>
+        <v>389</v>
       </c>
       <c r="B32" s="3">
         <v>1</v>
@@ -4663,7 +4540,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>439</v>
+        <v>390</v>
       </c>
       <c r="B33" s="3">
         <v>1</v>
@@ -4671,7 +4548,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>440</v>
+        <v>391</v>
       </c>
       <c r="B34" s="3">
         <v>1</v>
@@ -4679,7 +4556,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>441</v>
+        <v>392</v>
       </c>
       <c r="B35" s="3">
         <v>1</v>
@@ -4687,7 +4564,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>442</v>
+        <v>393</v>
       </c>
       <c r="B36" s="3">
         <v>1</v>
@@ -4695,7 +4572,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>398</v>
+        <v>349</v>
       </c>
       <c r="B37" s="3">
         <v>1</v>
@@ -4703,7 +4580,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>443</v>
+        <v>394</v>
       </c>
       <c r="B38" s="3">
         <v>1</v>
@@ -4711,7 +4588,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>403</v>
+        <v>354</v>
       </c>
       <c r="B39" s="3">
         <v>1</v>
@@ -4719,7 +4596,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>444</v>
+        <v>395</v>
       </c>
       <c r="B40" s="3">
         <v>1</v>
@@ -4727,7 +4604,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>405</v>
+        <v>356</v>
       </c>
       <c r="B41" s="3">
         <v>1</v>
@@ -4735,7 +4612,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>406</v>
+        <v>357</v>
       </c>
       <c r="B42" s="3">
         <v>1</v>
@@ -4743,7 +4620,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>445</v>
+        <v>396</v>
       </c>
       <c r="B43" s="3">
         <v>1</v>
@@ -4751,7 +4628,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>407</v>
+        <v>358</v>
       </c>
       <c r="B44" s="3">
         <v>1</v>
@@ -4759,7 +4636,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>408</v>
+        <v>359</v>
       </c>
       <c r="B45" s="3">
         <v>1</v>
@@ -4767,7 +4644,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>410</v>
+        <v>361</v>
       </c>
       <c r="B46" s="3">
         <v>1</v>
@@ -4775,7 +4652,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>409</v>
+        <v>360</v>
       </c>
       <c r="B47" s="3">
         <v>1</v>
@@ -4783,1239 +4660,1239 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="B48" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="B49" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="B50" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B51" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B52" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="B53" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B54" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="B55" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="B56" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="B57" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="B58" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="B59" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B60" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B61" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
         <v>411</v>
       </c>
-      <c r="B48" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="B62" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B63" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="B64" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B65" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B66" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B67" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="B68" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="B69" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="B70" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="B71" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B72" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="B73" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B74" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B75" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="B76" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="B77" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B78" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B79" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="B80" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="B81" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B82" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="B83" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="B49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+      <c r="B84" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B85" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B86" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B87" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B88" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B89" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="B90" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="B91" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B92" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B93" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B94" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="B50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>230</v>
-      </c>
-      <c r="B51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>231</v>
-      </c>
-      <c r="B52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>232</v>
-      </c>
-      <c r="B53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>233</v>
-      </c>
-      <c r="B54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>234</v>
-      </c>
-      <c r="B55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>235</v>
-      </c>
-      <c r="B56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>236</v>
-      </c>
-      <c r="B57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>237</v>
-      </c>
-      <c r="B58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>238</v>
-      </c>
-      <c r="B59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+      <c r="B95" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="B60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>240</v>
-      </c>
-      <c r="B61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>241</v>
-      </c>
-      <c r="B62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>242</v>
-      </c>
-      <c r="B63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>244</v>
-      </c>
-      <c r="B64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+      <c r="B96" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="B97" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B98" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="B99" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="B100" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B101" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="B102" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="B65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+      <c r="B103" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="B66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
+      <c r="B104" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="B67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>248</v>
-      </c>
-      <c r="B68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+      <c r="B105" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="B69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
+      <c r="B106" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="B107" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="B70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>252</v>
-      </c>
-      <c r="B71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+      <c r="B108" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="B72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+      <c r="B109" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="B73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
+      <c r="B110" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="B111" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="B74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
+      <c r="B112" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="B75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
+      <c r="B113" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="B76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
+      <c r="B114" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="B77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
+      <c r="B115" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="B78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
+      <c r="B116" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="B79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
+      <c r="B117" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="B80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
+      <c r="B118" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="B81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
+      <c r="B119" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="B82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
+      <c r="B120" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" s="6" t="s">
         <v>265</v>
       </c>
-      <c r="B83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
+      <c r="B121" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="B122" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="B123" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="B84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
+      <c r="B124" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="B85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>273</v>
-      </c>
-      <c r="B86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
+      <c r="B125" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="B126" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="B127" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="B128" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="B87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
+      <c r="B129" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="B88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
+      <c r="B130" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" s="6" t="s">
         <v>276</v>
       </c>
-      <c r="B89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
-        <v>277</v>
-      </c>
-      <c r="B90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
+      <c r="B131" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="B91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
+      <c r="B132" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="B92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
-        <v>280</v>
-      </c>
-      <c r="B93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
+      <c r="B133" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="B94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
+      <c r="B134" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="B135" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="B95">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
+      <c r="B136" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="B96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
+      <c r="B137" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="B97">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
+      <c r="B138" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="B98">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
-        <v>288</v>
-      </c>
-      <c r="B99">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
+      <c r="B139" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="B140" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" s="6" t="s">
         <v>290</v>
       </c>
-      <c r="B100">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
+      <c r="B141" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="B142" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
+      <c r="B143" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="B144" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="B102">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
+      <c r="B145" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="B103">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
-        <v>296</v>
-      </c>
-      <c r="B104">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
+      <c r="B146" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="B147" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="B105">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A106" t="s">
+      <c r="B148" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="B106">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
-        <v>300</v>
-      </c>
-      <c r="B107">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
+      <c r="B149" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="B150" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151" s="6" t="s">
         <v>302</v>
       </c>
-      <c r="B108">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
+      <c r="B151" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" s="6" t="s">
         <v>303</v>
       </c>
-      <c r="B109">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
+      <c r="B152" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153" s="6" t="s">
         <v>304</v>
       </c>
-      <c r="B110">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
+      <c r="B153" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154" s="6" t="s">
         <v>305</v>
       </c>
-      <c r="B111">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A112" t="s">
+      <c r="B154" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="B112">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
+      <c r="B155" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="B113">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
+      <c r="B156" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157" s="6" t="s">
         <v>308</v>
       </c>
-      <c r="B114">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
+      <c r="B157" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="B115">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
+      <c r="B158" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A159" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="B116">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
+      <c r="B159" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="B117">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
+      <c r="B160" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A161" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="B118">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
+      <c r="B161" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A162" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="B119">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A120" t="s">
+      <c r="B162" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A163" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="B120">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A121" t="s">
+      <c r="B163" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A164" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="B121">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A122" t="s">
+      <c r="B164" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A165" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="B122">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A123" t="s">
+      <c r="B165" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A166" s="6" t="s">
         <v>317</v>
       </c>
-      <c r="B123">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A124" t="s">
-        <v>318</v>
-      </c>
-      <c r="B124">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A125" t="s">
+      <c r="B166" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A167" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="B125">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A126" t="s">
+      <c r="B167" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A168" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="B126">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A127" t="s">
+      <c r="B168" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A169" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="B127">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A128" t="s">
+      <c r="B169" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A170" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="B170" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A171" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="B128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A129" t="s">
+      <c r="B171" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A172" s="6" t="s">
         <v>324</v>
       </c>
-      <c r="B129">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A130" t="s">
-        <v>325</v>
-      </c>
-      <c r="B130">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A131" t="s">
+      <c r="B172" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A173" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B173" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A174" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="B131">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A132" t="s">
+      <c r="B174" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A175" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="B132">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A133" t="s">
+      <c r="B175" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A176" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="B176" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A177" s="6" t="s">
         <v>330</v>
       </c>
-      <c r="B133">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A134" t="s">
+      <c r="B177" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A178" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="B134">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A135" t="s">
+      <c r="B178" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A179" s="6" t="s">
         <v>332</v>
       </c>
-      <c r="B135">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A136" t="s">
+      <c r="B179" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A180" s="6" t="s">
         <v>333</v>
       </c>
-      <c r="B136">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A137" t="s">
+      <c r="B180" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A181" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="B137">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A138" t="s">
+      <c r="B181" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A182" s="6" t="s">
         <v>335</v>
       </c>
-      <c r="B138">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A139" t="s">
-        <v>338</v>
-      </c>
-      <c r="B139">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A140" t="s">
+      <c r="B182" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A183" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="B183" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A184" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="B184" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A185" s="6" t="s">
         <v>339</v>
       </c>
-      <c r="B140">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A141" t="s">
+      <c r="B185" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A186" s="6" t="s">
         <v>340</v>
       </c>
-      <c r="B141">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A142" t="s">
+      <c r="B186" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A187" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="B142">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A143" t="s">
+      <c r="B187" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A188" s="6" t="s">
         <v>342</v>
       </c>
-      <c r="B143">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A144" t="s">
+      <c r="B188" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A189" s="6" t="s">
         <v>343</v>
       </c>
-      <c r="B144">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A145" t="s">
+      <c r="B189" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A190" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="B145">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A146" t="s">
+      <c r="B190" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A191" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="B191" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A192" s="6" t="s">
         <v>346</v>
       </c>
-      <c r="B146">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A147" t="s">
+      <c r="B192" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A193" s="6" t="s">
         <v>347</v>
       </c>
-      <c r="B147">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A148" t="s">
+      <c r="B193" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A194" s="6" t="s">
         <v>348</v>
       </c>
-      <c r="B148">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A149" t="s">
+      <c r="B194" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A195" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="B195" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A196" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B149">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A150" t="s">
+      <c r="B196" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A197" s="6" t="s">
         <v>351</v>
       </c>
-      <c r="B150">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A151" t="s">
+      <c r="B197" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A198" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="B151">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A152" t="s">
+      <c r="B198" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A199" s="6" t="s">
         <v>353</v>
       </c>
-      <c r="B152">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A153" t="s">
+      <c r="B199" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A200" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="B153">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A154" t="s">
+      <c r="B200" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A201" s="6" t="s">
         <v>355</v>
       </c>
-      <c r="B154">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A155" t="s">
-        <v>356</v>
-      </c>
-      <c r="B155">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A156" t="s">
-        <v>357</v>
-      </c>
-      <c r="B156">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A157" t="s">
-        <v>358</v>
-      </c>
-      <c r="B157">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A158" t="s">
-        <v>359</v>
-      </c>
-      <c r="B158">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A159" t="s">
-        <v>360</v>
-      </c>
-      <c r="B159">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A160" t="s">
-        <v>361</v>
-      </c>
-      <c r="B160">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A161" t="s">
-        <v>362</v>
-      </c>
-      <c r="B161">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A162" t="s">
-        <v>363</v>
-      </c>
-      <c r="B162">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A163" t="s">
-        <v>364</v>
-      </c>
-      <c r="B163">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A164" t="s">
-        <v>365</v>
-      </c>
-      <c r="B164">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A165" t="s">
-        <v>366</v>
-      </c>
-      <c r="B165">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A166" t="s">
-        <v>368</v>
-      </c>
-      <c r="B166">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A167" t="s">
-        <v>369</v>
-      </c>
-      <c r="B167">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A168" t="s">
-        <v>370</v>
-      </c>
-      <c r="B168">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A169" t="s">
-        <v>371</v>
-      </c>
-      <c r="B169">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A170" t="s">
-        <v>372</v>
-      </c>
-      <c r="B170">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A171" t="s">
-        <v>373</v>
-      </c>
-      <c r="B171">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A172" t="s">
-        <v>375</v>
-      </c>
-      <c r="B172">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A173" t="s">
-        <v>376</v>
-      </c>
-      <c r="B173">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A174" t="s">
-        <v>377</v>
-      </c>
-      <c r="B174">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A175" t="s">
-        <v>378</v>
-      </c>
-      <c r="B175">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A176" t="s">
-        <v>379</v>
-      </c>
-      <c r="B176">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A177" t="s">
-        <v>380</v>
-      </c>
-      <c r="B177">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A178" t="s">
-        <v>381</v>
-      </c>
-      <c r="B178">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A179" t="s">
-        <v>382</v>
-      </c>
-      <c r="B179">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A180" t="s">
-        <v>383</v>
-      </c>
-      <c r="B180">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A181" t="s">
-        <v>384</v>
-      </c>
-      <c r="B181">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A182" t="s">
-        <v>385</v>
-      </c>
-      <c r="B182">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A183" t="s">
-        <v>386</v>
-      </c>
-      <c r="B183">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A184" t="s">
-        <v>388</v>
-      </c>
-      <c r="B184">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A185" t="s">
-        <v>389</v>
-      </c>
-      <c r="B185">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A186" t="s">
-        <v>390</v>
-      </c>
-      <c r="B186">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A187" t="s">
-        <v>391</v>
-      </c>
-      <c r="B187">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A188" t="s">
-        <v>392</v>
-      </c>
-      <c r="B188">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A189" t="s">
-        <v>393</v>
-      </c>
-      <c r="B189">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A190" t="s">
-        <v>394</v>
-      </c>
-      <c r="B190">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A191" t="s">
-        <v>395</v>
-      </c>
-      <c r="B191">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A192" t="s">
-        <v>396</v>
-      </c>
-      <c r="B192">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A193" t="s">
-        <v>397</v>
-      </c>
-      <c r="B193">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A194" t="s">
-        <v>398</v>
-      </c>
-      <c r="B194">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A195" t="s">
-        <v>399</v>
-      </c>
-      <c r="B195">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A196" t="s">
-        <v>400</v>
-      </c>
-      <c r="B196">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A197" t="s">
-        <v>401</v>
-      </c>
-      <c r="B197">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A198" t="s">
-        <v>402</v>
-      </c>
-      <c r="B198">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A199" t="s">
-        <v>403</v>
-      </c>
-      <c r="B199">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A200" t="s">
-        <v>404</v>
-      </c>
-      <c r="B200">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A201" t="s">
-        <v>405</v>
-      </c>
-      <c r="B201">
+      <c r="B201" s="6">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B219">
-    <sortCondition descending="1" ref="B1:B219"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B220">
+    <sortCondition descending="1" ref="B1:B220"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Base de coletas não batia com a do github
</commit_message>
<xml_diff>
--- a/Coleta/base.xlsx
+++ b/Coleta/base.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alinsperedu-my.sharepoint.com/personal/jonasbp_al_insper_edu_br/Documents/2021.2/Ciência dos Dados/P1/Backup/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guigokuznietz/Desktop/P1-CDADOS2021.2/Coleta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="565" documentId="11_4A969315AC439293EE75102ED759FC45E12C451E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9344FBD-21EF-0045-98AD-101BFFF765DA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93F2183-BB38-D949-B8A3-4F70C90CCD20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="32000" windowHeight="15780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="419">
   <si>
     <t>Treinamento</t>
   </si>
@@ -1402,6 +1402,9 @@
   </si>
   <si>
     <t>“alexa toque uma playlist de shrek” advinha que disse isso 😂😂</t>
+  </si>
+  <si>
+    <t>Classificacao</t>
   </si>
 </sst>
 </file>
@@ -1832,8 +1835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B307"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A145" sqref="A145"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1844,6 +1847,9 @@
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -4276,8 +4282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="A107" sqref="A107"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4289,6 +4295,9 @@
       <c r="A1" s="1" t="s">
         <v>225</v>
       </c>
+      <c r="B1" t="s">
+        <v>418</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">

</xml_diff>